<commit_message>
removed activation and set filtered transplant as default
</commit_message>
<xml_diff>
--- a/data/livia/waiting_lists_real_comp.xlsx
+++ b/data/livia/waiting_lists_real_comp.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniroma2-my.sharepoint.com/personal/livia_simoncini_alumni_uniroma2_eu/Documents/Corsi/Attivi/PMCSN/Progetto/PMCSN_Project/data/livia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{173AB117-B007-4519-A928-0EECC1B8E3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5141EB15-0278-4C5A-B0B4-FC007289A265}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{173AB117-B007-4519-A928-0EECC1B8E3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAC97DE1-F475-4CD9-8121-496ED18A9EB6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{A135CD53-58D1-4A03-93CA-DA8D9B65F5BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{A135CD53-58D1-4A03-93CA-DA8D9B65F5BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
     <sheet name="Foglio4" sheetId="4" r:id="rId4"/>
+    <sheet name="Foglio5" sheetId="5" r:id="rId5"/>
+    <sheet name="Foglio6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="611">
   <si>
     <t>NO ACTIVATION/UNFILTERED MATCHING (5 YEARS)</t>
   </si>
@@ -1659,6 +1661,219 @@
   </si>
   <si>
     <t>+/-1.965841</t>
+  </si>
+  <si>
+    <t>+/-37.074934</t>
+  </si>
+  <si>
+    <t>+/-0.855463</t>
+  </si>
+  <si>
+    <t>+/-0.042452</t>
+  </si>
+  <si>
+    <t>+/-0.813687</t>
+  </si>
+  <si>
+    <t>+/-0.045388</t>
+  </si>
+  <si>
+    <t>+/-0.002273</t>
+  </si>
+  <si>
+    <t>+/-1.646060</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>+/-0.035491</t>
+  </si>
+  <si>
+    <t>+/-104.990402</t>
+  </si>
+  <si>
+    <t>+/-104.987444</t>
+  </si>
+  <si>
+    <t>+/-0.003008</t>
+  </si>
+  <si>
+    <t>+/-1506.093041</t>
+  </si>
+  <si>
+    <t>+/-1506.050608</t>
+  </si>
+  <si>
+    <t>inactive</t>
+  </si>
+  <si>
+    <t>+/-0.116432</t>
+  </si>
+  <si>
+    <t>+/-0.171744</t>
+  </si>
+  <si>
+    <t>+/-0.128719</t>
+  </si>
+  <si>
+    <t>+/-67.880114</t>
+  </si>
+  <si>
+    <t>+/-1.321790</t>
+  </si>
+  <si>
+    <t>+/-0.017274</t>
+  </si>
+  <si>
+    <t>+/-1.305377</t>
+  </si>
+  <si>
+    <t>+/-0.043686</t>
+  </si>
+  <si>
+    <t>+/-0.000562</t>
+  </si>
+  <si>
+    <t>+/-0.066517</t>
+  </si>
+  <si>
+    <t>+/-50.487706</t>
+  </si>
+  <si>
+    <t>+/-50.484564</t>
+  </si>
+  <si>
+    <t>+/-0.003196</t>
+  </si>
+  <si>
+    <t>+/-681.975746</t>
+  </si>
+  <si>
+    <t>+/-681.933342</t>
+  </si>
+  <si>
+    <t>+/-0.153815</t>
+  </si>
+  <si>
+    <t>+/-0.287501</t>
+  </si>
+  <si>
+    <t>+/-0.244670</t>
+  </si>
+  <si>
+    <t>+/-80.082395</t>
+  </si>
+  <si>
+    <t>+/-2.472485</t>
+  </si>
+  <si>
+    <t>+/-0.059812</t>
+  </si>
+  <si>
+    <t>+/-2.426585</t>
+  </si>
+  <si>
+    <t>+/-0.044075</t>
+  </si>
+  <si>
+    <t>+/-0.001030</t>
+  </si>
+  <si>
+    <t>+/-0.122835</t>
+  </si>
+  <si>
+    <t>+/-59.564205</t>
+  </si>
+  <si>
+    <t>+/-59.556774</t>
+  </si>
+  <si>
+    <t>+/-0.007568</t>
+  </si>
+  <si>
+    <t>+/-340.327071</t>
+  </si>
+  <si>
+    <t>+/-340.284729</t>
+  </si>
+  <si>
+    <t>+/-0.371597</t>
+  </si>
+  <si>
+    <t>+/-233.125899</t>
+  </si>
+  <si>
+    <t>+/-165.492741</t>
+  </si>
+  <si>
+    <t>+/-67.687489</t>
+  </si>
+  <si>
+    <t>+/-0.148082</t>
+  </si>
+  <si>
+    <t>+/-0.105046</t>
+  </si>
+  <si>
+    <t>+/-121.784280</t>
+  </si>
+  <si>
+    <t>+/-5.144559</t>
+  </si>
+  <si>
+    <t>+/-0.017862</t>
+  </si>
+  <si>
+    <t>+/-5.131710</t>
+  </si>
+  <si>
+    <t>+/-0.043279</t>
+  </si>
+  <si>
+    <t>+/-0.000155</t>
+  </si>
+  <si>
+    <t>+/-0.534304</t>
+  </si>
+  <si>
+    <t>+/-23.448919</t>
+  </si>
+  <si>
+    <t>+/-23.428190</t>
+  </si>
+  <si>
+    <t>+/-0.021073</t>
+  </si>
+  <si>
+    <t>+/-47.940166</t>
+  </si>
+  <si>
+    <t>+/-47.897706</t>
+  </si>
+  <si>
+    <t>+/-1.564580</t>
+  </si>
+  <si>
+    <t>+/-1334.574568</t>
+  </si>
+  <si>
+    <t>+/-1312.303977</t>
+  </si>
+  <si>
+    <t>+/-22.562496</t>
+  </si>
+  <si>
+    <t>+/-2.836987</t>
+  </si>
+  <si>
+    <t>+/-2.795683</t>
+  </si>
+  <si>
+    <t>OLD IMPL</t>
+  </si>
+  <si>
+    <t>NEW IMPL</t>
   </si>
 </sst>
 </file>
@@ -2080,8 +2295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C28B133F-C767-456A-9F55-0194E00F8498}">
   <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5425,7 +5640,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="A1:XFD1048576"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5626,7 +5841,7 @@
         <v>20.890470863013697</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H6:H14" si="1">AVERAGE(C6:C8)</f>
+        <f t="shared" ref="H8:H14" si="1">AVERAGE(C6:C8)</f>
         <v>4.16725105022831E-2</v>
       </c>
       <c r="I8">
@@ -5850,8 +6065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66ACCBBB-F9A6-4AD1-8D1B-67FEDC4C0F00}">
   <dimension ref="A1:T59"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:XFD59"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9194,7 +9409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E197E5A-77C8-47BD-A52F-E77C1545B835}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
@@ -9613,4 +9828,1060 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{698C3107-7B63-4ACC-B1CE-A47D6F7D53A5}">
+  <dimension ref="A1:T13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>90</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>77.786985999999999</v>
+      </c>
+      <c r="H2" t="s">
+        <v>540</v>
+      </c>
+      <c r="I2">
+        <v>8.3125599999999995</v>
+      </c>
+      <c r="J2" t="s">
+        <v>541</v>
+      </c>
+      <c r="K2">
+        <v>0.41555599999999998</v>
+      </c>
+      <c r="L2" t="s">
+        <v>542</v>
+      </c>
+      <c r="M2">
+        <v>7.8970039999999999</v>
+      </c>
+      <c r="N2" t="s">
+        <v>543</v>
+      </c>
+      <c r="O2">
+        <v>0.43556499999999998</v>
+      </c>
+      <c r="P2" t="s">
+        <v>544</v>
+      </c>
+      <c r="Q2">
+        <v>2.181E-2</v>
+      </c>
+      <c r="R2" t="s">
+        <v>545</v>
+      </c>
+      <c r="S2">
+        <v>2.1632999999999999E-2</v>
+      </c>
+      <c r="T2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>547</v>
+      </c>
+      <c r="C3">
+        <v>65111</v>
+      </c>
+      <c r="D3">
+        <v>4507</v>
+      </c>
+      <c r="E3">
+        <v>7440</v>
+      </c>
+      <c r="F3">
+        <v>48211</v>
+      </c>
+      <c r="G3">
+        <v>0.10414900000000001</v>
+      </c>
+      <c r="H3" t="s">
+        <v>548</v>
+      </c>
+      <c r="I3">
+        <v>794.275666</v>
+      </c>
+      <c r="J3" t="s">
+        <v>549</v>
+      </c>
+      <c r="K3">
+        <v>794.24679200000003</v>
+      </c>
+      <c r="L3" t="s">
+        <v>550</v>
+      </c>
+      <c r="M3">
+        <v>2.8874E-2</v>
+      </c>
+      <c r="N3" t="s">
+        <v>551</v>
+      </c>
+      <c r="O3">
+        <v>11382.754633</v>
+      </c>
+      <c r="P3" t="s">
+        <v>552</v>
+      </c>
+      <c r="Q3">
+        <v>11382.340878000001</v>
+      </c>
+      <c r="R3" t="s">
+        <v>553</v>
+      </c>
+      <c r="S3">
+        <v>2.1632999999999999E-2</v>
+      </c>
+      <c r="T3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>554</v>
+      </c>
+      <c r="C4">
+        <v>22140</v>
+      </c>
+      <c r="D4">
+        <v>5291</v>
+      </c>
+      <c r="E4">
+        <v>16849</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0.31869700000000001</v>
+      </c>
+      <c r="H4" t="s">
+        <v>555</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4">
+        <v>1.538262</v>
+      </c>
+      <c r="P4" t="s">
+        <v>556</v>
+      </c>
+      <c r="Q4">
+        <v>1.1245069999999999</v>
+      </c>
+      <c r="R4" t="s">
+        <v>557</v>
+      </c>
+      <c r="S4">
+        <v>2.1632999999999999E-2</v>
+      </c>
+      <c r="T4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>49</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>182.181321</v>
+      </c>
+      <c r="H5" t="s">
+        <v>558</v>
+      </c>
+      <c r="I5">
+        <v>13.260521000000001</v>
+      </c>
+      <c r="J5" t="s">
+        <v>559</v>
+      </c>
+      <c r="K5">
+        <v>0.15413499999999999</v>
+      </c>
+      <c r="L5" t="s">
+        <v>560</v>
+      </c>
+      <c r="M5">
+        <v>13.106386000000001</v>
+      </c>
+      <c r="N5" t="s">
+        <v>561</v>
+      </c>
+      <c r="O5">
+        <v>0.41864600000000002</v>
+      </c>
+      <c r="P5" t="s">
+        <v>562</v>
+      </c>
+      <c r="Q5">
+        <v>4.8910000000000004E-3</v>
+      </c>
+      <c r="R5" t="s">
+        <v>563</v>
+      </c>
+      <c r="S5">
+        <v>2.1632999999999999E-2</v>
+      </c>
+      <c r="T5" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>547</v>
+      </c>
+      <c r="C6">
+        <v>38774</v>
+      </c>
+      <c r="D6">
+        <v>2162</v>
+      </c>
+      <c r="E6">
+        <v>4257</v>
+      </c>
+      <c r="F6">
+        <v>21817</v>
+      </c>
+      <c r="G6">
+        <v>0.179982</v>
+      </c>
+      <c r="H6" t="s">
+        <v>564</v>
+      </c>
+      <c r="I6">
+        <v>378.01650899999999</v>
+      </c>
+      <c r="J6" t="s">
+        <v>565</v>
+      </c>
+      <c r="K6">
+        <v>377.98600900000002</v>
+      </c>
+      <c r="L6" t="s">
+        <v>566</v>
+      </c>
+      <c r="M6">
+        <v>3.0499999999999999E-2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>567</v>
+      </c>
+      <c r="O6">
+        <v>5126.227527</v>
+      </c>
+      <c r="P6" t="s">
+        <v>568</v>
+      </c>
+      <c r="Q6">
+        <v>5125.8137720000004</v>
+      </c>
+      <c r="R6" t="s">
+        <v>569</v>
+      </c>
+      <c r="S6">
+        <v>2.1632999999999999E-2</v>
+      </c>
+      <c r="T6" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>554</v>
+      </c>
+      <c r="C7">
+        <v>15620</v>
+      </c>
+      <c r="D7">
+        <v>3644</v>
+      </c>
+      <c r="E7">
+        <v>11973</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>0.44003199999999998</v>
+      </c>
+      <c r="H7" t="s">
+        <v>570</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7">
+        <v>2.758346</v>
+      </c>
+      <c r="P7" t="s">
+        <v>571</v>
+      </c>
+      <c r="Q7">
+        <v>2.3445909999999999</v>
+      </c>
+      <c r="R7" t="s">
+        <v>572</v>
+      </c>
+      <c r="S7">
+        <v>2.1632999999999999E-2</v>
+      </c>
+      <c r="T7" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>280.06782199999998</v>
+      </c>
+      <c r="H8" t="s">
+        <v>573</v>
+      </c>
+      <c r="I8">
+        <v>28.509810000000002</v>
+      </c>
+      <c r="J8" t="s">
+        <v>574</v>
+      </c>
+      <c r="K8">
+        <v>0.33326699999999998</v>
+      </c>
+      <c r="L8" t="s">
+        <v>575</v>
+      </c>
+      <c r="M8">
+        <v>28.176542999999999</v>
+      </c>
+      <c r="N8" t="s">
+        <v>576</v>
+      </c>
+      <c r="O8">
+        <v>0.41893200000000003</v>
+      </c>
+      <c r="P8" t="s">
+        <v>577</v>
+      </c>
+      <c r="Q8">
+        <v>5.1780000000000003E-3</v>
+      </c>
+      <c r="R8" t="s">
+        <v>578</v>
+      </c>
+      <c r="S8">
+        <v>2.1632999999999999E-2</v>
+      </c>
+      <c r="T8" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>547</v>
+      </c>
+      <c r="C9">
+        <v>19379</v>
+      </c>
+      <c r="D9">
+        <v>1424</v>
+      </c>
+      <c r="E9">
+        <v>2266</v>
+      </c>
+      <c r="F9">
+        <v>11086</v>
+      </c>
+      <c r="G9">
+        <v>0.35427500000000001</v>
+      </c>
+      <c r="H9" t="s">
+        <v>579</v>
+      </c>
+      <c r="I9">
+        <v>436.85981399999997</v>
+      </c>
+      <c r="J9" t="s">
+        <v>580</v>
+      </c>
+      <c r="K9">
+        <v>436.78825399999999</v>
+      </c>
+      <c r="L9" t="s">
+        <v>581</v>
+      </c>
+      <c r="M9">
+        <v>7.1561E-2</v>
+      </c>
+      <c r="N9" t="s">
+        <v>582</v>
+      </c>
+      <c r="O9">
+        <v>2523.1522599999998</v>
+      </c>
+      <c r="P9" t="s">
+        <v>583</v>
+      </c>
+      <c r="Q9">
+        <v>2522.7385049999998</v>
+      </c>
+      <c r="R9" t="s">
+        <v>584</v>
+      </c>
+      <c r="S9">
+        <v>2.1632999999999999E-2</v>
+      </c>
+      <c r="T9" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>554</v>
+      </c>
+      <c r="C10">
+        <v>6779</v>
+      </c>
+      <c r="D10">
+        <v>1543</v>
+      </c>
+      <c r="E10">
+        <v>5235</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>1.0412809999999999</v>
+      </c>
+      <c r="H10" t="s">
+        <v>585</v>
+      </c>
+      <c r="I10">
+        <v>1608.708447</v>
+      </c>
+      <c r="J10" t="s">
+        <v>586</v>
+      </c>
+      <c r="K10">
+        <v>1151.1091100000001</v>
+      </c>
+      <c r="L10" t="s">
+        <v>587</v>
+      </c>
+      <c r="M10">
+        <v>457.59933699999999</v>
+      </c>
+      <c r="N10" t="s">
+        <v>588</v>
+      </c>
+      <c r="O10">
+        <v>1.459271</v>
+      </c>
+      <c r="P10" t="s">
+        <v>589</v>
+      </c>
+      <c r="Q10">
+        <v>1.0455159999999999</v>
+      </c>
+      <c r="R10" t="s">
+        <v>590</v>
+      </c>
+      <c r="S10">
+        <v>2.1632999999999999E-2</v>
+      </c>
+      <c r="T10" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>495.42626000000001</v>
+      </c>
+      <c r="H11" t="s">
+        <v>591</v>
+      </c>
+      <c r="I11">
+        <v>53.80068</v>
+      </c>
+      <c r="J11" t="s">
+        <v>592</v>
+      </c>
+      <c r="K11">
+        <v>7.2725999999999999E-2</v>
+      </c>
+      <c r="L11" t="s">
+        <v>593</v>
+      </c>
+      <c r="M11">
+        <v>53.727953999999997</v>
+      </c>
+      <c r="N11" t="s">
+        <v>594</v>
+      </c>
+      <c r="O11">
+        <v>0.41434900000000002</v>
+      </c>
+      <c r="P11" t="s">
+        <v>595</v>
+      </c>
+      <c r="Q11">
+        <v>5.9400000000000002E-4</v>
+      </c>
+      <c r="R11" t="s">
+        <v>596</v>
+      </c>
+      <c r="S11">
+        <v>2.1632999999999999E-2</v>
+      </c>
+      <c r="T11" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>547</v>
+      </c>
+      <c r="C12">
+        <v>4143</v>
+      </c>
+      <c r="D12">
+        <v>209</v>
+      </c>
+      <c r="E12">
+        <v>363</v>
+      </c>
+      <c r="F12">
+        <v>1536</v>
+      </c>
+      <c r="G12">
+        <v>1.627327</v>
+      </c>
+      <c r="H12" t="s">
+        <v>597</v>
+      </c>
+      <c r="I12">
+        <v>178.609623</v>
+      </c>
+      <c r="J12" t="s">
+        <v>598</v>
+      </c>
+      <c r="K12">
+        <v>178.40624299999999</v>
+      </c>
+      <c r="L12" t="s">
+        <v>599</v>
+      </c>
+      <c r="M12">
+        <v>0.20338000000000001</v>
+      </c>
+      <c r="N12" t="s">
+        <v>600</v>
+      </c>
+      <c r="O12">
+        <v>363.51578499999999</v>
+      </c>
+      <c r="P12" t="s">
+        <v>601</v>
+      </c>
+      <c r="Q12">
+        <v>363.10203000000001</v>
+      </c>
+      <c r="R12" t="s">
+        <v>602</v>
+      </c>
+      <c r="S12">
+        <v>2.1632999999999999E-2</v>
+      </c>
+      <c r="T12" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>554</v>
+      </c>
+      <c r="C13">
+        <v>1781</v>
+      </c>
+      <c r="D13">
+        <v>405</v>
+      </c>
+      <c r="E13">
+        <v>1326</v>
+      </c>
+      <c r="F13">
+        <v>80</v>
+      </c>
+      <c r="G13">
+        <v>4.1024409999999998</v>
+      </c>
+      <c r="H13" t="s">
+        <v>603</v>
+      </c>
+      <c r="I13">
+        <v>6599.1483580000004</v>
+      </c>
+      <c r="J13" t="s">
+        <v>604</v>
+      </c>
+      <c r="K13">
+        <v>6446.6152460000003</v>
+      </c>
+      <c r="L13" t="s">
+        <v>605</v>
+      </c>
+      <c r="M13">
+        <v>152.53311199999999</v>
+      </c>
+      <c r="N13" t="s">
+        <v>606</v>
+      </c>
+      <c r="O13">
+        <v>16.909576000000001</v>
+      </c>
+      <c r="P13" t="s">
+        <v>607</v>
+      </c>
+      <c r="Q13">
+        <v>16.495820999999999</v>
+      </c>
+      <c r="R13" t="s">
+        <v>608</v>
+      </c>
+      <c r="S13">
+        <v>2.1632999999999999E-2</v>
+      </c>
+      <c r="T13" t="s">
+        <v>546</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C20371E-54CA-46E6-861D-71F1DA894B3E}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>609</v>
+      </c>
+      <c r="D1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <f>Foglio4!F3</f>
+        <v>2.1644397260273972E-2</v>
+      </c>
+      <c r="D2">
+        <f>Foglio5!I2/365</f>
+        <v>2.2774136986301367E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>547</v>
+      </c>
+      <c r="C3">
+        <f>Foglio4!F4</f>
+        <v>1.666442789041096</v>
+      </c>
+      <c r="D3">
+        <f>Foglio5!I3/365</f>
+        <v>2.1760977150684933</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>554</v>
+      </c>
+      <c r="C4">
+        <f>Foglio4!F5</f>
+        <v>14.465916775342466</v>
+      </c>
+      <c r="D4">
+        <f>Foglio5!I4/365</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <f>Foglio4!F6</f>
+        <v>3.6204065753424657E-2</v>
+      </c>
+      <c r="D5">
+        <f>Foglio5!I5/365</f>
+        <v>3.6330194520547948E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>547</v>
+      </c>
+      <c r="C6">
+        <f>Foglio4!F7</f>
+        <v>0.70419753972602739</v>
+      </c>
+      <c r="D6">
+        <f>Foglio5!I6/365</f>
+        <v>1.0356616684931506</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>554</v>
+      </c>
+      <c r="C7">
+        <f>Foglio4!F8</f>
+        <v>19.016048430136987</v>
+      </c>
+      <c r="D7">
+        <f>Foglio5!I7/365</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <f>Foglio4!F9</f>
+        <v>6.3253824657534249E-2</v>
+      </c>
+      <c r="D8">
+        <f>Foglio5!I8/365</f>
+        <v>7.8109068493150691E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>547</v>
+      </c>
+      <c r="C9">
+        <f>Foglio4!F10</f>
+        <v>0.84520046301369867</v>
+      </c>
+      <c r="D9">
+        <f>Foglio5!I9/365</f>
+        <v>1.1968762027397259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>554</v>
+      </c>
+      <c r="C10">
+        <f>Foglio4!F11</f>
+        <v>15.790427241095891</v>
+      </c>
+      <c r="D10">
+        <f>Foglio5!I10/365</f>
+        <v>4.4074204027397261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <f>Foglio4!F12</f>
+        <v>0.36181803013698632</v>
+      </c>
+      <c r="D11">
+        <f>Foglio5!I11/365</f>
+        <v>0.14739912328767124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>547</v>
+      </c>
+      <c r="C12">
+        <f>Foglio4!F13</f>
+        <v>0.28062932328767126</v>
+      </c>
+      <c r="D12">
+        <f>Foglio5!I12/365</f>
+        <v>0.48934143287671233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>554</v>
+      </c>
+      <c r="C13">
+        <f>Foglio4!F14</f>
+        <v>3.7646670630136985</v>
+      </c>
+      <c r="D13">
+        <f>Foglio5!I13/365</f>
+        <v>18.079858515068494</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f>AVERAGE(C2:C13)</f>
+        <v>4.7513708285388132</v>
+      </c>
+      <c r="D15">
+        <f>AVERAGE(D2:D13)</f>
+        <v>2.3058223716894979</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>